<commit_message>
Lagt til tabell for sammenligning av resultater fra Matlab og Python
</commit_message>
<xml_diff>
--- a/prosjektfiler/System_data_basecase_matlab.xlsx
+++ b/prosjektfiler/System_data_basecase_matlab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/IELET2118---Prosjekt-Lastflytanalyse/prosjektfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768922D2-D140-7545-8016-F0E4F4A047C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3219CDF-6EF3-8C42-895B-C4E09FD3BD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31800" yWindow="500" windowWidth="31800" windowHeight="23340" xr2:uid="{E6D3FD58-6DB6-4988-B229-9B990EF92238}"/>
+    <workbookView xWindow="-31800" yWindow="500" windowWidth="31800" windowHeight="23340" activeTab="1" xr2:uid="{E6D3FD58-6DB6-4988-B229-9B990EF92238}"/>
   </bookViews>
   <sheets>
     <sheet name="BranchData" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -124,14 +124,41 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-0 = Slack bus
-1 = PV-bus
-2 = PQ-bus</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">0 = Slack bus
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 = PV-bus
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2 = PQ-bus</t>
         </r>
       </text>
     </comment>
@@ -140,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>From Line</t>
   </si>
@@ -185,87 +212,6 @@
   </si>
   <si>
     <t>Q_gen</t>
-  </si>
-  <si>
-    <t>0.010177777777777777</t>
-  </si>
-  <si>
-    <t>0.10941111111111111</t>
-  </si>
-  <si>
-    <t>0.005633095539372249</t>
-  </si>
-  <si>
-    <t>0.008355555555555555</t>
-  </si>
-  <si>
-    <t>0.08982222222222222</t>
-  </si>
-  <si>
-    <t>0.00462455004979032</t>
-  </si>
-  <si>
-    <t>0.021244444444444444</t>
-  </si>
-  <si>
-    <t>0.22837777777777776</t>
-  </si>
-  <si>
-    <t>0.011758164488296662</t>
-  </si>
-  <si>
-    <t>0.004033333333333333</t>
-  </si>
-  <si>
-    <t>0.044366666666666665</t>
-  </si>
-  <si>
-    <t>0.003865949671727993</t>
-  </si>
-  <si>
-    <t>0.015822222222222224</t>
-  </si>
-  <si>
-    <t>0.2531555555555556</t>
-  </si>
-  <si>
-    <t>0.022949711325591874</t>
-  </si>
-  <si>
-    <t>0.01208888888888889</t>
-  </si>
-  <si>
-    <t>0.19342222222222225</t>
-  </si>
-  <si>
-    <t>0.017534610900452215</t>
-  </si>
-  <si>
-    <t>0.021955555555555555</t>
-  </si>
-  <si>
-    <t>0.2360222222222222</t>
-  </si>
-  <si>
-    <t>0.012151743215938392</t>
-  </si>
-  <si>
-    <t>0.04702222222222223</t>
-  </si>
-  <si>
-    <t>0.5054888888888889</t>
-  </si>
-  <si>
-    <t>0.02602539336530935</t>
-  </si>
-  <si>
-    <t>0.05186666666666667</t>
-  </si>
-  <si>
-    <t>0.5575666666666667</t>
-  </si>
-  <si>
-    <t>0.028706648447368633</t>
   </si>
 </sst>
 </file>
@@ -656,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81158F8-AC87-45D5-9D87-5F767982CA33}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -690,14 +636,14 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
+      <c r="C2" s="3">
+        <v>1.0177777777777701E-2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.109411111111111</v>
+      </c>
+      <c r="E2" s="3">
+        <v>5.6330955393722399E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -707,14 +653,14 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
+      <c r="C3" s="3">
+        <v>8.3555555555555501E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8.9822222222222206E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4.6245500497903201E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -724,14 +670,14 @@
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
+      <c r="C4" s="3">
+        <v>2.1244444444444399E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.22837777777777701</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.1758164488296601E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -741,14 +687,14 @@
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>26</v>
+      <c r="C5" s="3">
+        <v>4.0333333333333297E-3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4.4366666666666603E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.8659496717279901E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -758,14 +704,14 @@
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
+      <c r="C6" s="3">
+        <v>1.5822222222222199E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.25315555555555502</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.2949711325591801E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -775,14 +721,14 @@
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>32</v>
+      <c r="C7" s="3">
+        <v>1.20888888888888E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.193422222222222</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.7534610900452201E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -792,14 +738,14 @@
       <c r="B8">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>35</v>
+      <c r="C8" s="3">
+        <v>2.1955555555555499E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.23602222222222199</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.21517432159383E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -809,14 +755,14 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>38</v>
+      <c r="C9" s="3">
+        <v>4.7022222222222201E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.50548888888888799</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2.6025393365309301E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -826,14 +772,14 @@
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>41</v>
+      <c r="C10" s="3">
+        <v>5.1866666666666603E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.55756666666666599</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2.8706648447368598E-2</v>
       </c>
     </row>
   </sheetData>
@@ -847,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C983FE4D-AF19-4D14-8B95-201C762457E9}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -894,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>L2*1.02</f>
@@ -927,7 +873,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>L2*1.033</f>
@@ -954,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f>L2*1.029</f>
@@ -981,7 +927,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>L2*0.985</f>
@@ -1008,10 +954,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -1034,10 +980,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -1060,10 +1006,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -1086,10 +1032,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>

</xml_diff>